<commit_message>
Starting With new db
</commit_message>
<xml_diff>
--- a/openBackend/openApi/csv_file/Open_Course.xlsx
+++ b/openBackend/openApi/csv_file/Open_Course.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,12 +453,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20PICS378</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Mithun</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -466,7 +466,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>_5D02HIS</t>
+          <t>_5D01COM</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -476,12 +476,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20PICS378</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Mithun</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -489,7 +489,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>_5D01BOT</t>
+          <t>_5D05CSC</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -499,12 +499,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20PICS378</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Mithun</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -512,22 +512,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>_5D04MAL</t>
+          <t>_5D04CHE</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20PICS378</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Mithun</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -535,22 +535,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>_5D03CHE</t>
+          <t>_5D01BOT</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20PICS378</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Mithun</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -558,22 +558,22 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>_5D03MAL</t>
+          <t>_5D03CHE</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20PICS378</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Mithun</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -581,559 +581,559 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>_5D05POL</t>
+          <t>_5D03COM</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>_5D01COM</t>
+          <t>_5D05PHY</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>_5D01ECO</t>
+          <t>_5D03COM</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>_5D01HIS</t>
+          <t>_5D03CHE</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>_5D04CHE</t>
+          <t>_5D01COM</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>_5D03COM</t>
+          <t>_5D02STA</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>_5D03HIS</t>
+          <t>_5D05PED</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>_5D03BOT</t>
+          <t>_5D02CSC</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>_5D04MAT</t>
+          <t>_5D01POL</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>_5D05SKT</t>
+          <t>_5D05POL</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>_5D02MAT</t>
+          <t>_5D04STA</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>_5D05PED</t>
+          <t>_5D05CSC</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>_5D03PHY</t>
+          <t>_5D01HIS</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>_5D01POL</t>
+          <t>_5D02HIS</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>_5D02SKT</t>
+          <t>_5D03MAL</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>_5D05PHY</t>
+          <t>_5D04MAL</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>NA20PICS05</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>gopika</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>_5D03ZLG</t>
+          <t>_5D01BOT</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>NA20PICS67</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Amal K</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>_5D03CHE</t>
+          <t>_5D03BOT</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>NA20PICS67</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Amal K</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>_5D01BOT</t>
+          <t>_5D04CHE</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>NA20PICS67</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Amal K</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>_5D03BOT</t>
+          <t>_5D02MAT</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>NA20PICS67</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Amal K</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>_5D04CHE</t>
+          <t>_5D04MAT</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>NA20PICS67</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Amal K</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>_5D01COM</t>
+          <t>_5D03PHY</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>NA20PICS10</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>AMAL</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1094</v>
+        <v>1118</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>_5D03COM</t>
+          <t>_5D02ZLG</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>NA20PICS10</t>
+          <t>NA20AECR012</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>AMAL</t>
+          <t>Amna Jasmine Karayil</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1094</v>
+        <v>1118</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>_5D01ECO</t>
+          <t>_5D03ZLG</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>_5D01BOT</t>
+          <t>_5D05PHY</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1143,20 +1143,20 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>_5D02MAT</t>
+          <t>_5D03COM</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1166,296 +1166,296 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>_5D01COM</t>
+          <t>_5D03CHE</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>_5D04CHE</t>
+          <t>_5D01COM</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>_5D01ECO</t>
+          <t>_5D02STA</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>_5D03CHE</t>
+          <t>_5D05PED</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>_5D02HIS</t>
+          <t>_5D04STA</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>_5D01POL</t>
+          <t>_5D01BOT</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>_5D04ECO</t>
+          <t>_5D03BOT</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>_5D03COM</t>
+          <t>_5D04CHE</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>_5D01HIS</t>
+          <t>_5D02CSC</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>_5D03MAL</t>
+          <t>_5D05CSC</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>_5D05PED</t>
+          <t>_5D01HIS</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>_5D04MAL</t>
+          <t>_5D02HIS</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>_5D05SKT</t>
+          <t>_5D02MAT</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1465,20 +1465,20 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>_5D05PHY</t>
+          <t>_5D04MAT</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1488,20 +1488,20 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>_5D03HIS</t>
+          <t>_5D03PHY</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1511,20 +1511,20 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>_5D04MAT</t>
+          <t>_5D01POL</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1534,16 +1534,16 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1557,20 +1557,20 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>_5D03PHY</t>
+          <t>_5D02SKT</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1580,20 +1580,20 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>_5D04STA</t>
+          <t>_5D05SKT</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -1603,20 +1603,20 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>NA20PICS23</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>_5D02SKT</t>
+          <t>_5D02ZLG</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -1626,691 +1626,1082 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR015</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Fathima E K</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1005</v>
+        <v>1112</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>_5D01BOT</t>
+          <t>_5D03ZLG</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>_5D03BOT</t>
+          <t>_5D01COM</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>_5D01COM</t>
+          <t>_5D05PHY</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>_5D04CHE</t>
+          <t>_5D03CHE</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>_5D01ECO</t>
+          <t>_5D03COM</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>_5D03CHE</t>
+          <t>_5D04MAL</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>_5D02HIS</t>
+          <t>_5D04MAT</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>_5D01POL</t>
+          <t>_5D01BOT</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>_5D04ECO</t>
+          <t>_5D03BOT</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>_5D03COM</t>
+          <t>_5D04CHE</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>_5D01HIS</t>
+          <t>_5D02CSC</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>_5D03MAL</t>
+          <t>_5D05CSC</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>_5D05PED</t>
+          <t>_5D01HIS</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>_5D04MAL</t>
+          <t>_5D02HIS</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>_5D05SKT</t>
+          <t>_5D03HIS</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>_5D05PHY</t>
+          <t>_5D02STA</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>_5D03HIS</t>
+          <t>_5D04STA</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>_5D04MAT</t>
+          <t>_5D03ZLG</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>_5D05POL</t>
+          <t>_5D03PHY</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>_5D03PHY</t>
+          <t>_5D02MAT</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>_5D04STA</t>
+          <t>_5D03MAL</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Arjun</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1005</v>
+        <v>1065</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>_5D02SKT</t>
+          <t>_5D05POL</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>NA20PICS34</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Raju</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>960</v>
+        <v>1065</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>_5D03CHE</t>
+          <t>_5D05PED</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>NA20PICS34</t>
+          <t>NA20AECR032</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Raju</t>
+          <t>Amreenaysha</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>960</v>
+        <v>1065</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>_5D01COM</t>
+          <t>_5D01POL</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20ACER029</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>TEST</t>
+          <t>Abina Rajan</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>419</v>
+        <v>909</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>_5D01BOT</t>
+          <t>_5D01POL</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20ACER029</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>TEST</t>
+          <t>Abina Rajan</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>419</v>
+        <v>909</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>_5D03MAL</t>
+          <t>_5D02MAT</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20ACER029</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>TEST</t>
+          <t>Abina Rajan</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>419</v>
+        <v>909</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>_5D04ECO</t>
+          <t>_5D05POL</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20ACER029</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>TEST</t>
+          <t>Abina Rajan</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>419</v>
+        <v>909</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>_5D02HIS</t>
+          <t>_5D01COM</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20ACER029</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>TEST</t>
+          <t>Abina Rajan</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>419</v>
+        <v>909</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>_5D01ECO</t>
+          <t>_5D03COM</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>NA20PICS11</t>
+          <t>NA20ACER029</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>TEST</t>
+          <t>Abina Rajan</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>419</v>
+        <v>909</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>_5D03COM</t>
+          <t>_5D02CSC</t>
         </is>
       </c>
       <c r="E82" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>909</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>_5D04MAT</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>909</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>_5D05CSC</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>909</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>_5D02ZLG</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>909</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>_5D05PHY</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>909</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>_5D03CHE</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>909</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>_5D03PHY</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>909</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>_5D04CHE</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>909</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>_5D01BOT</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>909</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>_5D03ZLG</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>909</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>_5D03BOT</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>909</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>_5D02HIS</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>909</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>_5D01HIS</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>909</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>_5D03MAL</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>909</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>_5D03HIS</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>909</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>_5D04STA</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
         <v>22</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>909</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>_5D02STA</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>NA20ACER029</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Abina Rajan</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>909</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>_5D05SKT</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>